<commit_message>
Add lat, lng to the cities and plot them on the map in the instances entity report.
</commit_message>
<xml_diff>
--- a/public/data/advanced_data_example_v20151104.xlsx
+++ b/public/data/advanced_data_example_v20151104.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="root_hospital_cities" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>cityName</t>
   </si>
@@ -213,13 +213,31 @@
   </si>
   <si>
     <t>root_hospital</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>latitude in degrees</t>
+  </si>
+  <si>
+    <t>longitude in degrees</t>
+  </si>
+  <si>
+    <t>decimal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,6 +270,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -289,9 +314,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -637,27 +664,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="3">
+        <v>40.712783999999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-74.005941000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>37.151164999999999</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-88.731998000000004</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +891,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -905,113 +948,141 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
       </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
       </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>61</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1030,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
altered emx documentation, mref added to advanced example (data)
</commit_message>
<xml_diff>
--- a/public/data/advanced_data_example_v20151104.xlsx
+++ b/public/data/advanced_data_example_v20151104.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="679" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="root_hospital_cities" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
   <si>
     <t>cityName</t>
   </si>
   <si>
-    <t>new york</t>
-  </si>
-  <si>
     <t>metropolis</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>disease</t>
   </si>
   <si>
-    <t>john doe</t>
-  </si>
-  <si>
     <t>john</t>
   </si>
   <si>
@@ -68,15 +62,9 @@
     <t>none</t>
   </si>
   <si>
-    <t>jane doe</t>
-  </si>
-  <si>
     <t>jane</t>
   </si>
   <si>
-    <t>pape doe</t>
-  </si>
-  <si>
     <t>papa</t>
   </si>
   <si>
@@ -228,6 +216,30 @@
   </si>
   <si>
     <t>decimal</t>
+  </si>
+  <si>
+    <t>new_york</t>
+  </si>
+  <si>
+    <t>john_doe</t>
+  </si>
+  <si>
+    <t>jane_doe</t>
+  </si>
+  <si>
+    <t>papa_doe</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>john_doe, jane_doe</t>
+  </si>
+  <si>
+    <t>mref</t>
+  </si>
+  <si>
+    <t>children of a patient</t>
   </si>
 </sst>
 </file>
@@ -297,8 +309,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -320,7 +338,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -328,6 +346,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -335,6 +356,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -666,7 +690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -675,15 +701,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3">
         <v>40.712783999999999</v>
@@ -694,7 +720,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>37.151164999999999</v>
@@ -715,86 +741,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="G15" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -812,71 +844,71 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -891,10 +923,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -908,25 +940,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -934,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -943,43 +975,43 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -988,107 +1020,123 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1102,7 +1150,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1114,74 +1162,73 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1206,37 +1253,36 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>